<commit_message>
Ajuste Historico de Gastos
</commit_message>
<xml_diff>
--- a/WebContent/resources/files/Archivo Plano Presupuesto Nómina.xlsx
+++ b/WebContent/resources/files/Archivo Plano Presupuesto Nómina.xlsx
@@ -12,12 +12,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Usuarios!$A$5:$F$5</definedName>
   </definedNames>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Nombre</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>Escriba una clasificación(Gasto, Inversion, Órdenes)</t>
+  </si>
+  <si>
+    <t>Observación</t>
   </si>
 </sst>
 </file>
@@ -126,12 +129,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -434,21 +436,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="11" width="6.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="7.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="11" width="6.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="7.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -468,7 +471,7 @@
       <c r="M1"/>
       <c r="N1"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
@@ -488,7 +491,7 @@
       <c r="M2"/>
       <c r="N2"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
@@ -508,7 +511,7 @@
       <c r="M3"/>
       <c r="N3"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4"/>
       <c r="B4"/>
       <c r="C4"/>
@@ -524,7 +527,7 @@
       <c r="M4"/>
       <c r="N4"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -567,38 +570,9 @@
       <c r="N5" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
+      <c r="O5" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>